<commit_message>
Added doors to board
</commit_message>
<xml_diff>
--- a/Board.xlsx
+++ b/Board.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="31">
   <si>
     <t>w</t>
   </si>
@@ -49,6 +49,66 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>DR</t>
+  </si>
+  <si>
+    <t>CU</t>
+  </si>
+  <si>
+    <t>LL</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>KR</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>OL</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>BU</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>KD</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>HU</t>
+  </si>
+  <si>
+    <t>KL</t>
   </si>
 </sst>
 </file>
@@ -545,7 +605,7 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -564,7 +624,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
@@ -573,7 +633,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>0</v>
@@ -594,7 +654,7 @@
         <v>7</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>0</v>
@@ -615,7 +675,7 @@
         <v>2</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>0</v>
@@ -630,7 +690,7 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -757,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>2</v>
@@ -782,7 +842,7 @@
       </c>
       <c r="Y3" s="3"/>
       <c r="Z3">
-        <f t="shared" ref="Z3:Z23" si="0">Z2+1</f>
+        <f t="shared" ref="Z3:Z22" si="0">Z2+1</f>
         <v>2</v>
       </c>
     </row>
@@ -979,7 +1039,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>7</v>
@@ -1000,10 +1060,10 @@
         <v>2</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="U6" s="2" t="s">
         <v>2</v>
@@ -1125,7 +1185,7 @@
         <v>6</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>0</v>
@@ -1304,7 +1364,7 @@
         <v>10</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>0</v>
@@ -1341,7 +1401,7 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
@@ -1629,10 +1689,10 @@
         <v>0</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="T14" s="1" t="s">
         <v>0</v>
@@ -1647,7 +1707,7 @@
         <v>4</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="Y14" s="3"/>
       <c r="Z14">
@@ -1669,7 +1729,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>0</v>
@@ -1678,7 +1738,7 @@
         <v>9</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>0</v>
@@ -1696,7 +1756,7 @@
         <v>10</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="O15" s="2" t="s">
         <v>10</v>
@@ -1936,7 +1996,7 @@
         <v>0</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>8</v>
@@ -2106,7 +2166,7 @@
         <v>8</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="T20" s="1" t="s">
         <v>0</v>
@@ -2222,7 +2282,7 @@
         <v>3</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>0</v>
@@ -2243,7 +2303,7 @@
         <v>9</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>0</v>
@@ -2270,7 +2330,7 @@
         <v>0</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="V22" s="2" t="s">
         <v>4</v>
@@ -2323,7 +2383,7 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <f t="shared" ref="C24:Y24" si="1">B24+1</f>
+        <f t="shared" ref="C24:X24" si="1">B24+1</f>
         <v>2</v>
       </c>
       <c r="D24">

</xml_diff>

<commit_message>
Added cluelegend.txt and converted layout to cluelayout.csv
</commit_message>
<xml_diff>
--- a/Board.xlsx
+++ b/Board.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="18195" windowHeight="7995"/>
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="31">
   <si>
-    <t>w</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>KL</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
@@ -605,83 +605,83 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Y1" s="3"/>
       <c r="Z1">
@@ -690,76 +690,76 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="P2" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Y2" s="3"/>
       <c r="Z2">
@@ -769,76 +769,76 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="P3" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Y3" s="3"/>
       <c r="Z3">
@@ -848,76 +848,76 @@
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="P4" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Y4" s="3"/>
       <c r="Z4">
@@ -927,76 +927,76 @@
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="P5" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Y5" s="3"/>
       <c r="Z5">
@@ -1006,76 +1006,76 @@
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="P6" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Y6" s="3"/>
       <c r="Z6">
@@ -1085,76 +1085,76 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Y7" s="3"/>
       <c r="Z7">
@@ -1164,76 +1164,76 @@
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Y8" s="3"/>
       <c r="Z8">
@@ -1243,76 +1243,76 @@
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Y9" s="3"/>
       <c r="Z9">
@@ -1322,76 +1322,76 @@
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="P10" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V10" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Y10" s="3"/>
       <c r="Z10">
@@ -1401,76 +1401,76 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V11" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Y11" s="3"/>
       <c r="Z11">
@@ -1480,76 +1480,76 @@
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V12" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Y12" s="3"/>
       <c r="Z12">
@@ -1559,76 +1559,76 @@
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Y13" s="3"/>
       <c r="Z13">
@@ -1638,76 +1638,76 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y14" s="3"/>
       <c r="Z14">
@@ -1717,76 +1717,76 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="O15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y15" s="3"/>
       <c r="Z15">
@@ -1796,76 +1796,76 @@
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y16" s="3"/>
       <c r="Z16">
@@ -1875,76 +1875,76 @@
     </row>
     <row r="17" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y17" s="3"/>
       <c r="Z17">
@@ -1954,76 +1954,76 @@
     </row>
     <row r="18" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y18" s="3"/>
       <c r="Z18">
@@ -2033,76 +2033,76 @@
     </row>
     <row r="19" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y19" s="3"/>
       <c r="Z19">
@@ -2112,76 +2112,76 @@
     </row>
     <row r="20" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y20" s="3"/>
       <c r="Z20">
@@ -2191,76 +2191,76 @@
     </row>
     <row r="21" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y21" s="3"/>
       <c r="Z21">
@@ -2270,76 +2270,76 @@
     </row>
     <row r="22" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y22" s="3"/>
       <c r="Z22">
@@ -2467,7 +2467,7 @@
         <v>22</v>
       </c>
       <c r="X24">
-        <f t="shared" si="1"/>
+        <f>W24+1</f>
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added my test squares to board
</commit_message>
<xml_diff>
--- a/Board.xlsx
+++ b/Board.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="18195" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13770" windowHeight="7305"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="35">
   <si>
     <t>X</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>Number of Doors: 23</t>
+  </si>
+  <si>
+    <t>Door</t>
+  </si>
+  <si>
+    <t>Tested in testDoorDirection()</t>
+  </si>
+  <si>
+    <t>Tested for correct initial</t>
   </si>
 </sst>
 </file>
@@ -124,7 +136,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,6 +167,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -168,12 +198,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z24"/>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -632,7 +665,7 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="6" t="s">
         <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -653,7 +686,7 @@
       <c r="N1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="6" t="s">
         <v>24</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -674,7 +707,7 @@
       <c r="U1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="5" t="s">
         <v>14</v>
       </c>
       <c r="W1" s="1" t="s">
@@ -689,7 +722,7 @@
       </c>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -807,7 +840,7 @@
       <c r="M3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="O3" s="2" t="s">
@@ -816,7 +849,7 @@
       <c r="P3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="R3" s="2" t="s">
@@ -850,13 +883,13 @@
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -1038,7 +1071,7 @@
       <c r="K6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="M6" s="2" t="s">
@@ -1053,16 +1086,16 @@
       <c r="P6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="Q6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="S6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="T6" s="6" t="s">
         <v>25</v>
       </c>
       <c r="U6" s="2" t="s">
@@ -1105,7 +1138,7 @@
       <c r="G7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -1184,7 +1217,7 @@
       <c r="G8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="6" t="s">
         <v>20</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -1205,7 +1238,7 @@
       <c r="N8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="O8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="P8" s="1" t="s">
@@ -1363,7 +1396,7 @@
       <c r="N10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="O10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="P10" s="1" t="s">
@@ -1378,7 +1411,7 @@
       <c r="S10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="T10" s="4" t="s">
+      <c r="T10" s="7" t="s">
         <v>0</v>
       </c>
       <c r="U10" s="4" t="s">
@@ -1400,7 +1433,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1688,10 +1721,10 @@
       <c r="Q14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R14" s="2" t="s">
+      <c r="R14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="S14" s="2" t="s">
+      <c r="S14" s="6" t="s">
         <v>11</v>
       </c>
       <c r="T14" s="1" t="s">
@@ -1706,7 +1739,7 @@
       <c r="W14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="X14" s="2" t="s">
+      <c r="X14" s="6" t="s">
         <v>26</v>
       </c>
       <c r="Y14" s="3"/>
@@ -1728,16 +1761,16 @@
       <c r="D15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="2" t="s">
+      <c r="G15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>28</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -1755,7 +1788,7 @@
       <c r="M15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="N15" s="5" t="s">
         <v>23</v>
       </c>
       <c r="O15" s="2" t="s">
@@ -1959,7 +1992,7 @@
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1995,7 +2028,7 @@
       <c r="N18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="O18" s="6" t="s">
         <v>27</v>
       </c>
       <c r="P18" s="2" t="s">
@@ -2165,7 +2198,7 @@
       <c r="R20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="S20" s="2" t="s">
+      <c r="S20" s="6" t="s">
         <v>13</v>
       </c>
       <c r="T20" s="1" t="s">
@@ -2281,7 +2314,7 @@
       <c r="D22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -2302,7 +2335,7 @@
       <c r="K22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="L22" s="6" t="s">
         <v>15</v>
       </c>
       <c r="M22" s="1" t="s">
@@ -2323,13 +2356,13 @@
       <c r="R22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="S22" s="2" t="s">
+      <c r="S22" s="7" t="s">
         <v>7</v>
       </c>
       <c r="T22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="U22" s="2" t="s">
+      <c r="U22" s="7" t="s">
         <v>12</v>
       </c>
       <c r="V22" s="2" t="s">
@@ -2338,7 +2371,7 @@
       <c r="W22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="X22" s="2" t="s">
+      <c r="X22" s="5" t="s">
         <v>3</v>
       </c>
       <c r="Y22" s="3"/>
@@ -2383,7 +2416,7 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <f t="shared" ref="C24:X24" si="1">B24+1</f>
+        <f t="shared" ref="C24:W24" si="1">B24+1</f>
         <v>2</v>
       </c>
       <c r="D24">
@@ -2469,6 +2502,29 @@
       <c r="X24">
         <f>W24+1</f>
         <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>